<commit_message>
Updated Sprint Burn down chart with Sprint 1 data.
</commit_message>
<xml_diff>
--- a/Planning and Design/SprintBurnDown.xlsx
+++ b/Planning and Design/SprintBurnDown.xlsx
@@ -1,27 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr updateLinks="always"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\gcu.edu\home\HomeDrive\andrew.silver\profile\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/19cdf6dfaf774916/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="80" documentId="8_{0EBC6F26-9873-4339-AB5E-ACFE727B1FD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8D883B6D-B525-4CCA-A86B-47FE5E004645}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="12885"/>
+    <workbookView xWindow="2798" yWindow="1763" windowWidth="20490" windowHeight="13094" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Burn Down Chart" sheetId="1" r:id="rId1"/>
     <sheet name="How To Use" sheetId="2" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -31,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
   <si>
     <t>Task</t>
   </si>
@@ -72,20 +79,12 @@
     <t>Estimate</t>
   </si>
   <si>
-    <t>Project Title:
-Release #:
-Sprint #:</t>
-  </si>
-  <si>
     <t>User Story ID</t>
   </si>
   <si>
     <t>Assigned To</t>
   </si>
   <si>
-    <t>Team Member</t>
-  </si>
-  <si>
     <t>Task 1</t>
   </si>
   <si>
@@ -104,24 +103,9 @@
     <t>Task 6</t>
   </si>
   <si>
-    <t>Task 7</t>
-  </si>
-  <si>
-    <t>Task 8</t>
-  </si>
-  <si>
-    <t>Task 9</t>
-  </si>
-  <si>
-    <t>Task 10</t>
-  </si>
-  <si>
     <t>User Story</t>
   </si>
   <si>
-    <t>As a(n) &lt;actor&gt; I would like to &lt;description&gt;</t>
-  </si>
-  <si>
     <t>Step 1</t>
   </si>
   <si>
@@ -174,12 +158,59 @@
   </si>
   <si>
     <t>After each Daily Standup each Team Member should review the Burn Down Chart to ensure your Sprint will be delivered on time</t>
+  </si>
+  <si>
+    <t>Project Title: Minesweeper
+Release #: 1.0
+Sprint #: 1</t>
+  </si>
+  <si>
+    <t>M2-1</t>
+  </si>
+  <si>
+    <t>M2-2</t>
+  </si>
+  <si>
+    <t>M2-3</t>
+  </si>
+  <si>
+    <t>M2-4</t>
+  </si>
+  <si>
+    <t>M2-6</t>
+  </si>
+  <si>
+    <t>M2-5</t>
+  </si>
+  <si>
+    <t>I would like to setup the database so we can save data</t>
+  </si>
+  <si>
+    <t>I would like to create login and registration controllers</t>
+  </si>
+  <si>
+    <t>I would like to create models for user and registration</t>
+  </si>
+  <si>
+    <t>I would like to create views that are consumed by controllers</t>
+  </si>
+  <si>
+    <t>I would like to insure that controllers and views validate data</t>
+  </si>
+  <si>
+    <t>I would like to update design documentation</t>
+  </si>
+  <si>
+    <t>Shawn</t>
+  </si>
+  <si>
+    <t>Richard</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -321,7 +352,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -350,7 +381,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -382,89 +412,90 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:strRef>
-              <c:f>[1]Sheet1!$F$5:$O$5</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>Day 10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Day 9</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Day 8</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Day 7</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Day 6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Day 5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Day 4</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Day 3</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Day 2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Day 1</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:strLit>
+              <c:ptCount val="10"/>
+              <c:pt idx="0">
+                <c:v>Day 10</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>Day 9</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>Day 8</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>Day 7</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>Day 6</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>Day 5</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>Day 4</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>Day 3</c:v>
+              </c:pt>
+              <c:pt idx="8">
+                <c:v>Day 2</c:v>
+              </c:pt>
+              <c:pt idx="9">
+                <c:v>Day 1</c:v>
+              </c:pt>
+            </c:strLit>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>[1]Sheet1!$F$19:$O$19</c:f>
+              <c:f>'Burn Down Chart'!$G$14:$P$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>27</c:v>
+                  <c:v>8.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24</c:v>
+                  <c:v>7.1999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>21</c:v>
+                  <c:v>6.2999999999999989</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18</c:v>
+                  <c:v>5.3999999999999986</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15</c:v>
+                  <c:v>4.4999999999999982</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12</c:v>
+                  <c:v>3.5999999999999983</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9</c:v>
+                  <c:v>2.6999999999999984</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6</c:v>
+                  <c:v>1.7999999999999985</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3</c:v>
+                  <c:v>0.89999999999999847</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>-1.5543122344752192E-15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BD09-4309-AE89-D2DA3CBC5AC9}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -489,89 +520,90 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:strRef>
-              <c:f>[1]Sheet1!$F$5:$O$5</c:f>
-              <c:strCache>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>Day 10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Day 9</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Day 8</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Day 7</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Day 6</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Day 5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Day 4</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Day 3</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Day 2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Day 1</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:strLit>
+              <c:ptCount val="10"/>
+              <c:pt idx="0">
+                <c:v>Day 10</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>Day 9</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>Day 8</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>Day 7</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>Day 6</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>Day 5</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>Day 4</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>Day 3</c:v>
+              </c:pt>
+              <c:pt idx="8">
+                <c:v>Day 2</c:v>
+              </c:pt>
+              <c:pt idx="9">
+                <c:v>Day 1</c:v>
+              </c:pt>
+            </c:strLit>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>[1]Sheet1!$F$20:$O$20</c:f>
+              <c:f>'Burn Down Chart'!$G$15:$P$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>29</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>27</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>21</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>17</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-BD09-4309-AE89-D2DA3CBC5AC9}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -622,7 +654,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -654,7 +685,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -672,120 +709,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-      <sheetName val="Sheet2"/>
-      <sheetName val="Sheet3"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="5">
-          <cell r="F5" t="str">
-            <v>Day 10</v>
-          </cell>
-          <cell r="G5" t="str">
-            <v>Day 9</v>
-          </cell>
-          <cell r="H5" t="str">
-            <v>Day 8</v>
-          </cell>
-          <cell r="I5" t="str">
-            <v>Day 7</v>
-          </cell>
-          <cell r="J5" t="str">
-            <v>Day 6</v>
-          </cell>
-          <cell r="K5" t="str">
-            <v>Day 5</v>
-          </cell>
-          <cell r="L5" t="str">
-            <v>Day 4</v>
-          </cell>
-          <cell r="M5" t="str">
-            <v>Day 3</v>
-          </cell>
-          <cell r="N5" t="str">
-            <v>Day 2</v>
-          </cell>
-          <cell r="O5" t="str">
-            <v>Day 1</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="F19">
-            <v>27</v>
-          </cell>
-          <cell r="G19">
-            <v>24</v>
-          </cell>
-          <cell r="H19">
-            <v>21</v>
-          </cell>
-          <cell r="I19">
-            <v>18</v>
-          </cell>
-          <cell r="J19">
-            <v>15</v>
-          </cell>
-          <cell r="K19">
-            <v>12</v>
-          </cell>
-          <cell r="L19">
-            <v>9</v>
-          </cell>
-          <cell r="M19">
-            <v>6</v>
-          </cell>
-          <cell r="N19">
-            <v>3</v>
-          </cell>
-          <cell r="O19">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="F20">
-            <v>29</v>
-          </cell>
-          <cell r="G20">
-            <v>27</v>
-          </cell>
-          <cell r="H20">
-            <v>21</v>
-          </cell>
-          <cell r="I20">
-            <v>21</v>
-          </cell>
-          <cell r="J20">
-            <v>17</v>
-          </cell>
-          <cell r="K20">
-            <v>17</v>
-          </cell>
-          <cell r="L20">
-            <v>11</v>
-          </cell>
-          <cell r="M20">
-            <v>6</v>
-          </cell>
-          <cell r="N20">
-            <v>6</v>
-          </cell>
-          <cell r="O20">
-            <v>0</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1050,24 +973,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="13" style="8" customWidth="1"/>
     <col min="3" max="3" width="21" style="8" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" customWidth="1"/>
+    <col min="4" max="4" width="20.86328125" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="48" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="13" t="s">
-        <v>13</v>
+        <v>40</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -1076,7 +999,7 @@
       <c r="F1" s="14"/>
       <c r="G1" s="14"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A2" s="1"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -1096,19 +1019,19 @@
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A3" s="1"/>
       <c r="B3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>12</v>
@@ -1146,77 +1069,81 @@
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
     </row>
-    <row r="4" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A4" s="1"/>
-      <c r="B4" s="7">
-        <v>1</v>
+      <c r="B4" s="7" t="s">
+        <v>41</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="F4" s="4">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="G4" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H4" s="4">
         <v>0</v>
       </c>
       <c r="I4" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J4" s="4">
         <v>0</v>
       </c>
       <c r="K4" s="4">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L4" s="4">
         <v>0</v>
       </c>
       <c r="M4" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N4" s="4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="O4" s="4">
         <v>0</v>
       </c>
       <c r="P4" s="4">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A5" s="1"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="10"/>
+      <c r="B5" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>48</v>
+      </c>
       <c r="D5" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="F5" s="4">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G5" s="4">
         <v>0</v>
       </c>
       <c r="H5" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I5" s="4">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J5" s="4">
         <v>0</v>
@@ -1228,7 +1155,7 @@
         <v>0</v>
       </c>
       <c r="M5" s="4">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="N5" s="4">
         <v>0</v>
@@ -1242,18 +1169,22 @@
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A6" s="1"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="10"/>
+      <c r="B6" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>49</v>
+      </c>
       <c r="D6" s="9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="F6" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" s="4">
         <v>0</v>
@@ -1288,18 +1219,22 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A7" s="1"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="10"/>
+      <c r="B7" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>50</v>
+      </c>
       <c r="D7" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>16</v>
+        <v>54</v>
       </c>
       <c r="F7" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G7" s="4">
         <v>0</v>
@@ -1334,22 +1269,22 @@
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
     </row>
-    <row r="8" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A8" s="1"/>
-      <c r="B8" s="7">
+      <c r="B8" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" s="4">
         <v>2</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="4">
-        <v>0</v>
       </c>
       <c r="G8" s="4">
         <v>0</v>
@@ -1384,18 +1319,22 @@
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A9" s="1"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="10"/>
+      <c r="B9" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>52</v>
+      </c>
       <c r="D9" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>16</v>
+        <v>54</v>
       </c>
       <c r="F9" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9" s="4">
         <v>0</v>
@@ -1430,16 +1369,12 @@
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A10" s="1"/>
       <c r="B10" s="7"/>
       <c r="C10" s="10"/>
-      <c r="D10" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="D10" s="9"/>
+      <c r="E10" s="3"/>
       <c r="F10" s="4">
         <v>0</v>
       </c>
@@ -1476,20 +1411,12 @@
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
     </row>
-    <row r="11" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A11" s="1"/>
-      <c r="B11" s="7">
-        <v>3</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="3"/>
       <c r="F11" s="4">
         <v>0</v>
       </c>
@@ -1526,20 +1453,12 @@
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
     </row>
-    <row r="12" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A12" s="1"/>
-      <c r="B12" s="7">
-        <v>4</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="3"/>
       <c r="F12" s="4">
         <v>0</v>
       </c>
@@ -1576,20 +1495,12 @@
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
     </row>
-    <row r="13" spans="1:18" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A13" s="1"/>
-      <c r="B13" s="7">
-        <v>5</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="3"/>
       <c r="F13" s="4">
         <v>0</v>
       </c>
@@ -1626,7 +1537,7 @@
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A14" s="1"/>
       <c r="B14" s="12" t="s">
         <v>10</v>
@@ -1636,52 +1547,52 @@
       <c r="E14" s="12"/>
       <c r="F14" s="4">
         <f>SUM(F4:F13)</f>
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="G14" s="4">
         <f>F14-$F$14/10</f>
-        <v>27</v>
+        <v>8.1</v>
       </c>
       <c r="H14" s="4">
         <f t="shared" ref="H14:P14" si="0">G14-$F$14/10</f>
-        <v>24</v>
+        <v>7.1999999999999993</v>
       </c>
       <c r="I14" s="4">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>6.2999999999999989</v>
       </c>
       <c r="J14" s="4">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>5.3999999999999986</v>
       </c>
       <c r="K14" s="4">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>4.4999999999999982</v>
       </c>
       <c r="L14" s="4">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>3.5999999999999983</v>
       </c>
       <c r="M14" s="4">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>2.6999999999999984</v>
       </c>
       <c r="N14" s="4">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>1.7999999999999985</v>
       </c>
       <c r="O14" s="4">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0.89999999999999847</v>
       </c>
       <c r="P14" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-1.5543122344752192E-15</v>
       </c>
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A15" s="1"/>
       <c r="B15" s="12" t="s">
         <v>11</v>
@@ -1691,52 +1602,52 @@
       <c r="E15" s="12"/>
       <c r="F15" s="4">
         <f>SUM(F4:F13)</f>
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="G15" s="4">
         <f t="shared" ref="G15:P15" si="1">F15 - SUM(G4:G13)</f>
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="H15" s="4">
         <f t="shared" si="1"/>
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="I15" s="4">
         <f t="shared" si="1"/>
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="J15" s="4">
         <f t="shared" si="1"/>
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="K15" s="4">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="L15" s="4">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="M15" s="4">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="N15" s="4">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="O15" s="4">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="P15" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A16" s="1"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -1756,7 +1667,7 @@
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A17" s="1"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -1776,7 +1687,7 @@
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A18" s="1"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -1796,7 +1707,7 @@
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A19" s="1"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -1816,7 +1727,7 @@
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A20" s="1"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -1836,7 +1747,7 @@
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A21" s="1"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -1856,7 +1767,7 @@
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A22" s="1"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -1876,7 +1787,7 @@
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A23" s="1"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -1896,7 +1807,7 @@
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A24" s="1"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -1916,7 +1827,7 @@
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A25" s="1"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
@@ -1936,7 +1847,7 @@
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A26" s="1"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -1956,7 +1867,7 @@
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A27" s="1"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -1976,7 +1887,7 @@
       <c r="Q27" s="1"/>
       <c r="R27" s="1"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A28" s="1"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -1996,7 +1907,7 @@
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A29" s="1"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -2016,7 +1927,7 @@
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A30" s="1"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -2036,7 +1947,7 @@
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A31" s="1"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -2056,7 +1967,7 @@
       <c r="Q31" s="1"/>
       <c r="R31" s="1"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A32" s="1"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
@@ -2076,7 +1987,7 @@
       <c r="Q32" s="1"/>
       <c r="R32" s="1"/>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A33" s="1"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -2096,7 +2007,7 @@
       <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A34" s="1"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
@@ -2116,7 +2027,7 @@
       <c r="Q34" s="1"/>
       <c r="R34" s="1"/>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A35" s="1"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
@@ -2136,7 +2047,7 @@
       <c r="Q35" s="1"/>
       <c r="R35" s="1"/>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A36" s="1"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -2156,7 +2067,7 @@
       <c r="Q36" s="1"/>
       <c r="R36" s="1"/>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A37" s="1"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
@@ -2192,148 +2103,148 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" customWidth="1"/>
+    <col min="1" max="1" width="10.86328125" customWidth="1"/>
     <col min="2" max="2" width="228" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="11" t="s">
+    </row>
+    <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="11" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+      <c r="B5" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="11" t="s">
+    </row>
+    <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="11" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
+      <c r="B6" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="11" t="s">
+    </row>
+    <row r="7" spans="1:2" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="11" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="11" t="s">
+      <c r="B7" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="11" t="s">
+    </row>
+    <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="11" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="11" t="s">
+      <c r="B8" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="11" t="s">
+    </row>
+    <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="11" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="11" t="s">
+      <c r="B9" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
     </row>
-    <row r="11" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="11"/>
       <c r="B11" s="11"/>
     </row>
-    <row r="12" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="11"/>
       <c r="B12" s="11"/>
     </row>
-    <row r="13" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="11"/>
       <c r="B13" s="11"/>
     </row>
-    <row r="14" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="11"/>
       <c r="B14" s="11"/>
     </row>
-    <row r="15" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="11"/>
       <c r="B15" s="11"/>
     </row>
-    <row r="16" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="11"/>
       <c r="B16" s="11"/>
     </row>
-    <row r="17" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="11"/>
       <c r="B17" s="11"/>
     </row>
-    <row r="18" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="11"/>
       <c r="B18" s="11"/>
     </row>
-    <row r="19" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="11"/>
       <c r="B19" s="11"/>
     </row>
-    <row r="20" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="11"/>
       <c r="B20" s="11"/>
     </row>
-    <row r="21" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="11"/>
       <c r="B21" s="11"/>
     </row>
-    <row r="22" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="11"/>
       <c r="B22" s="11"/>
     </row>
-    <row r="23" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="11"/>
       <c r="B23" s="11"/>
     </row>
-    <row r="24" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="11"/>
       <c r="B24" s="11"/>
     </row>
@@ -2352,21 +2263,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
-  <xsnLocation/>
-  <cached>True</cached>
-  <openByDefault>False</openByDefault>
-  <xsnScope/>
-</customXsn>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events"/>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B9FDC2B66788A044965A7B8958E6244A" ma:contentTypeVersion="1251" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6c2c36359d71eb747fbb188f75fc8d29">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="d6188da8-f31e-469a-aed4-03a23c44e36a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="08acee74153637279a480e75df712a71" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2555,7 +2451,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -2573,26 +2469,25 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B20B8EA-C8C4-49B1-8280-945BA6550F81}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA975265-C41C-4191-AC8E-A5AD70B8A3C6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="d6188da8-f31e-469a-aed4-03a23c44e36a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D14C1044-F523-4937-BF47-727729F19EA1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA975265-C41C-4191-AC8E-A5AD70B8A3C6}"/>
-</file>
-
-<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90C1BE12-9AF4-4D82-8933-6D42A4A8E2C9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>

</xml_diff>

<commit_message>
Updated Burn Down Chart for Fradet
</commit_message>
<xml_diff>
--- a/Planning and Design/SprintBurnDown.xlsx
+++ b/Planning and Design/SprintBurnDown.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr updateLinks="always"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/19cdf6dfaf774916/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shawn\source\CST-323\CST-247-Project\Planning and Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="80" documentId="8_{0EBC6F26-9873-4339-AB5E-ACFE727B1FD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8D883B6D-B525-4CCA-A86B-47FE5E004645}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0D7F58E-A5EE-4ABD-91EC-C45A839EDB7E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2798" yWindow="1763" windowWidth="20490" windowHeight="13094" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2798" yWindow="1763" windowWidth="20490" windowHeight="13094" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Burn Down Chart" sheetId="1" r:id="rId1"/>
@@ -569,31 +569,31 @@
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -976,8 +976,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1090,7 +1090,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I4" s="4">
         <v>0</v>
@@ -1140,7 +1140,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" s="4">
         <v>0</v>
@@ -1193,7 +1193,7 @@
         <v>0</v>
       </c>
       <c r="I6" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" s="4">
         <v>0</v>
@@ -1610,39 +1610,39 @@
       </c>
       <c r="H15" s="4">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I15" s="4">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="J15" s="4">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="K15" s="4">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="L15" s="4">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="M15" s="4">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="N15" s="4">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="O15" s="4">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="P15" s="4">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
@@ -2106,7 +2106,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -2254,12 +2254,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2452,18 +2452,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D6E300D-687F-49DD-9C99-AC5EA1BE3BF7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90C1BE12-9AF4-4D82-8933-6D42A4A8E2C9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="30a82cfc-8d0b-455e-b705-4035c60ff9fd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2488,18 +2497,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90C1BE12-9AF4-4D82-8933-6D42A4A8E2C9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D6E300D-687F-49DD-9C99-AC5EA1BE3BF7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="30a82cfc-8d0b-455e-b705-4035c60ff9fd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>